<commit_message>
feat(agent): add html analysis to agenttools
</commit_message>
<xml_diff>
--- a/output/custos_por_colaborador.xlsx
+++ b/output/custos_por_colaborador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Salário</t>
+          <t>Salario</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Custo Unimed</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Custo Gympass</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Custo GitHub</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Custo Google Workspace</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Custo Claude</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Custo Total</t>
         </is>
@@ -471,12 +491,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>177d2a03-dd33-5953-8650-1de95414461f</t>
+          <t>00a0d290-74eb-5793-8df7-98f4280eb295</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Adolfo Moreira</t>
+          <t>Antônia Pires</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,13 +505,25 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3384.960765580439</v>
+        <v>9976.53102463056</v>
       </c>
       <c r="F2" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G2" t="n">
-        <v>3474.960765580439</v>
+        <v>90</v>
+      </c>
+      <c r="H2" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I2" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J2" t="n">
+        <v>150</v>
+      </c>
+      <c r="K2" t="n">
+        <v>11213.28102463056</v>
       </c>
     </row>
     <row r="3">
@@ -500,12 +532,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>41cf3515-ef53-595d-a1e6-4d127d75533b</t>
+          <t>06be0738-b15f-5d07-892b-d45971647c79</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Adriana Nogueira</t>
+          <t>Danilo Brandão</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -514,13 +546,25 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3719.103451680459</v>
+        <v>9095.090151715545</v>
       </c>
       <c r="F3" t="n">
-        <v>90</v>
+        <v>855.8</v>
       </c>
       <c r="G3" t="n">
-        <v>3809.103451680459</v>
+        <v>90</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10348.02015171554</v>
       </c>
     </row>
     <row r="4">
@@ -529,27 +573,39 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>39f92dc0-2ae9-596f-a160-35025eebbff1</t>
+          <t>0eab9fc6-2c73-5288-af73-b13876c87b62</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Afonso Barros</t>
+          <t>Catarina Chaves</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>8962.729721841501</v>
+        <v>3490.64446620121</v>
       </c>
       <c r="F4" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G4" t="n">
-        <v>9052.729721841501</v>
+        <v>90</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J4" t="n">
+        <v>10</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4332.76446620121</v>
       </c>
     </row>
     <row r="5">
@@ -558,27 +614,39 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>b96b9339-e1b9-5d20-b70d-67a8bdb16875</t>
+          <t>1202a201-05dd-5f81-bff7-762f946c273e</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Alan Esteves</t>
+          <t>Ariane Teixeira</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8059.789738823023</v>
+        <v>8271.84079484528</v>
       </c>
       <c r="F5" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G5" t="n">
-        <v>8149.789738823023</v>
+        <v>90</v>
+      </c>
+      <c r="H5" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I5" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J5" t="n">
+        <v>150</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9597.590794845279</v>
       </c>
     </row>
     <row r="6">
@@ -587,12 +655,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a4b3dbb1-86f1-5d25-95a4-82a6c3076da1</t>
+          <t>1539ddc4-5241-5e9d-9086-cc8aea7dcbb1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Alberto da Luz</t>
+          <t>Augusto Nunes</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -601,13 +669,25 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7364.526801321949</v>
+        <v>4963.54282637831</v>
       </c>
       <c r="F6" t="n">
-        <v>90</v>
+        <v>560.7</v>
       </c>
       <c r="G6" t="n">
-        <v>7454.526801321949</v>
+        <v>90</v>
+      </c>
+      <c r="H6" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I6" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J6" t="n">
+        <v>150</v>
+      </c>
+      <c r="K6" t="n">
+        <v>6316.00282637831</v>
       </c>
     </row>
     <row r="7">
@@ -616,12 +696,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>282b242b-4e87-51f2-a5ff-d141bd8825c8</t>
+          <t>17533122-8361-509c-9e67-8887db2e0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Alessandra Dias</t>
+          <t>Diana Azevedo</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -630,13 +710,23 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5318.987724937523</v>
+        <v>6993.13850131002</v>
       </c>
       <c r="F7" t="n">
-        <v>90</v>
+        <v>-328.28</v>
       </c>
       <c r="G7" t="n">
-        <v>5408.987724937523</v>
+        <v>90</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>7051.98850131002</v>
       </c>
     </row>
     <row r="8">
@@ -645,12 +735,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ca2f5a2d-c388-5837-ae1f-93173331ba9a</t>
+          <t>177d2a03-dd33-5953-8650-1de95414461f</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Alexandre da Mata</t>
+          <t>Adolfo Moreira</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -659,13 +749,25 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>9551.21905794158</v>
+        <v>3384.960765580439</v>
       </c>
       <c r="F8" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G8" t="n">
-        <v>9641.21905794158</v>
+        <v>90</v>
+      </c>
+      <c r="H8" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J8" t="n">
+        <v>150</v>
+      </c>
+      <c r="K8" t="n">
+        <v>4710.710765580439</v>
       </c>
     </row>
     <row r="9">
@@ -674,27 +776,39 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>c4998a9b-cc38-5851-9223-7cf43ea91c36</t>
+          <t>25f4b46b-119b-54b7-a5fa-03827e5ed16f</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Alice Farias</t>
+          <t>Carolina Salgado</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>8284.136836853117</v>
+        <v>3266.657357480083</v>
       </c>
       <c r="F9" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G9" t="n">
-        <v>8374.136836853117</v>
+        <v>164</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J9" t="n">
+        <v>10</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4102.547357480083</v>
       </c>
     </row>
     <row r="10">
@@ -703,12 +817,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>73f85436-2fc0-5fc4-840f-f9f03c4fc92b</t>
+          <t>282b242b-4e87-51f2-a5ff-d141bd8825c8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Aline da Rocha</t>
+          <t>Alessandra Dias</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -717,13 +831,25 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1315.118209620667</v>
+        <v>5318.987724937523</v>
       </c>
       <c r="F10" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G10" t="n">
-        <v>1405.118209620667</v>
+        <v>90</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J10" t="n">
+        <v>150</v>
+      </c>
+      <c r="K10" t="n">
+        <v>6301.107724937523</v>
       </c>
     </row>
     <row r="11">
@@ -732,12 +858,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>d4d9f427-c9cd-5935-a88d-60bb469e7c89</t>
+          <t>2bc2241b-333d-5e89-9b7c-7c6524872c01</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Álvaro da Paz</t>
+          <t>Camila Dantas</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -746,13 +872,23 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1223.312552727439</v>
+        <v>1280.596453813949</v>
       </c>
       <c r="F11" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G11" t="n">
-        <v>1313.312552727439</v>
+        <v>90</v>
+      </c>
+      <c r="H11" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I11" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>2367.346453813949</v>
       </c>
     </row>
     <row r="12">
@@ -761,12 +897,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>442868a8-fabc-5568-a849-51f72b08b3c7</t>
+          <t>2c297031-afd1-540c-a226-32291c3b420d</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Amanda Pinto</t>
+          <t>Eduardo Portela</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -775,13 +911,25 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>4021.833629163991</v>
+        <v>1728.629771639805</v>
       </c>
       <c r="F12" t="n">
-        <v>90</v>
+        <v>560.7</v>
       </c>
       <c r="G12" t="n">
-        <v>4111.833629163992</v>
+        <v>117</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J12" t="n">
+        <v>50</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2753.459771639805</v>
       </c>
     </row>
     <row r="13">
@@ -790,12 +938,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>56f44ead-fafa-5e60-a0a7-e51d81a79de8</t>
+          <t>2f144455-ef5b-5852-8ccb-71bbb361384b</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Amélia Ribeiro</t>
+          <t>Bruno Castro</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -804,13 +952,23 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>5244.623025188975</v>
+        <v>4610.394047610112</v>
       </c>
       <c r="F13" t="n">
-        <v>117</v>
+        <v>364.76</v>
       </c>
       <c r="G13" t="n">
-        <v>5361.623025188975</v>
+        <v>90</v>
+      </c>
+      <c r="H13" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I13" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>5616.914047610113</v>
       </c>
     </row>
     <row r="14">
@@ -819,12 +977,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ea3147dc-902e-5ded-88e8-10514c53e142</t>
+          <t>361c4b67-5ca5-59d1-998e-08ceca3ebc57</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Ana Melo</t>
+          <t>Bárbara Neves</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -833,13 +991,25 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8057.257421621038</v>
+        <v>4587.767886848967</v>
       </c>
       <c r="F14" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G14" t="n">
-        <v>8147.257421621038</v>
+        <v>117</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J14" t="n">
+        <v>150</v>
+      </c>
+      <c r="K14" t="n">
+        <v>5516.657886848967</v>
       </c>
     </row>
     <row r="15">
@@ -848,12 +1018,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>f9e02392-bc91-5868-91d5-4a90ccc2cbbf</t>
+          <t>39f92dc0-2ae9-596f-a160-35025eebbff1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Anderson Aragão</t>
+          <t>Afonso Barros</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -862,13 +1032,25 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>9712.728285382607</v>
+        <v>8962.729721841501</v>
       </c>
       <c r="F15" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G15" t="n">
-        <v>9802.728285382607</v>
+        <v>90</v>
+      </c>
+      <c r="H15" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I15" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J15" t="n">
+        <v>150</v>
+      </c>
+      <c r="K15" t="n">
+        <v>10086.3097218415</v>
       </c>
     </row>
     <row r="16">
@@ -877,27 +1059,39 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>631aa093-f502-5229-8a89-b7392dcec06c</t>
+          <t>3d13f1ba-db27-5fa6-9587-1c539c366638</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>André da Rosa</t>
+          <t>Celso Mourão</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>7487.999892436921</v>
+        <v>257.9421561647101</v>
       </c>
       <c r="F16" t="n">
-        <v>90</v>
+        <v>404.91</v>
       </c>
       <c r="G16" t="n">
-        <v>7577.999892436921</v>
+        <v>90</v>
+      </c>
+      <c r="H16" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I16" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1314.61215616471</v>
       </c>
     </row>
     <row r="17">
@@ -906,12 +1100,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6156d6e1-5c40-5ed7-9144-6856fbfbb067</t>
+          <t>3f4a1eeb-c287-57d9-8407-78ea76ba96ea</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Andreia Peixoto</t>
+          <t>Cristina Meireles</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -920,13 +1114,25 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>8029.53768092652</v>
+        <v>6183.77422031294</v>
       </c>
       <c r="F17" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G17" t="n">
-        <v>8119.53768092652</v>
+        <v>90</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J17" t="n">
+        <v>10</v>
+      </c>
+      <c r="K17" t="n">
+        <v>6945.66422031294</v>
       </c>
     </row>
     <row r="18">
@@ -935,27 +1141,39 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>f08290a7-3372-5637-9244-a80f8bc9ee3c</t>
+          <t>41cf3515-ef53-595d-a1e6-4d127d75533b</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ângela Rezende</t>
+          <t>Adriana Nogueira</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2036.514997025348</v>
+        <v>3719.103451680459</v>
       </c>
       <c r="F18" t="n">
-        <v>90</v>
+        <v>855.8</v>
       </c>
       <c r="G18" t="n">
-        <v>2126.514997025348</v>
+        <v>90</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J18" t="n">
+        <v>150</v>
+      </c>
+      <c r="K18" t="n">
+        <v>5112.033451680459</v>
       </c>
     </row>
     <row r="19">
@@ -964,12 +1182,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>c4fd9f54-9504-52b3-9fca-ab39c50dc07f</t>
+          <t>442868a8-fabc-5568-a849-51f72b08b3c7</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Anselmo Novaes</t>
+          <t>Amanda Pinto</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -978,13 +1196,25 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1108.340345861018</v>
+        <v>4021.833629163991</v>
       </c>
       <c r="F19" t="n">
-        <v>90</v>
+        <v>848.05</v>
       </c>
       <c r="G19" t="n">
-        <v>1198.340345861018</v>
+        <v>90</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J19" t="n">
+        <v>150</v>
+      </c>
+      <c r="K19" t="n">
+        <v>5407.013629163991</v>
       </c>
     </row>
     <row r="20">
@@ -993,27 +1223,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>00a0d290-74eb-5793-8df7-98f4280eb295</t>
+          <t>4b86c62c-6ddf-539d-ac69-cc6cc522386a</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Antônia Pires</t>
+          <t>Diego Figueiredo</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>9976.53102463056</v>
+        <v>490.174359132607</v>
       </c>
       <c r="F20" t="n">
-        <v>90</v>
+        <v>622.41</v>
       </c>
       <c r="G20" t="n">
-        <v>10066.53102463056</v>
+        <v>90</v>
+      </c>
+      <c r="H20" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I20" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>1754.344359132607</v>
       </c>
     </row>
     <row r="21">
@@ -1022,12 +1262,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ce6652c4-e8d1-5805-81c2-2fdc603f51b0</t>
+          <t>52f4cadd-4009-5089-b7fa-65f6e4ab2887</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Antônio Viana</t>
+          <t>Carlos Magalhães</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1036,13 +1276,25 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>3295.032751492262</v>
+        <v>8837.775201541868</v>
       </c>
       <c r="F21" t="n">
-        <v>117</v>
+        <v>364.76</v>
       </c>
       <c r="G21" t="n">
-        <v>3412.032751492262</v>
+        <v>90</v>
+      </c>
+      <c r="H21" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I21" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J21" t="n">
+        <v>10</v>
+      </c>
+      <c r="K21" t="n">
+        <v>9854.295201541867</v>
       </c>
     </row>
     <row r="22">
@@ -1051,27 +1303,39 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1202a201-05dd-5f81-bff7-762f946c273e</t>
+          <t>56f44ead-fafa-5e60-a0a7-e51d81a79de8</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Ariane Teixeira</t>
+          <t>Amélia Ribeiro</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>8271.84079484528</v>
+        <v>5244.623025188975</v>
       </c>
       <c r="F22" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G22" t="n">
-        <v>8361.84079484528</v>
+        <v>117</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J22" t="n">
+        <v>150</v>
+      </c>
+      <c r="K22" t="n">
+        <v>6342.743025188975</v>
       </c>
     </row>
     <row r="23">
@@ -1080,27 +1344,39 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>71019c83-dffc-5bad-8c7f-bd61b699add5</t>
+          <t>607d85fb-c6b1-57ad-8bbe-b1a93fa57349</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arthur Gusmão</t>
+          <t>Benedito Silveira</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>5288.260196934793</v>
+        <v>1362.231969577253</v>
       </c>
       <c r="F23" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G23" t="n">
-        <v>5378.260196934793</v>
+        <v>90</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J23" t="n">
+        <v>150</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2344.351969577253</v>
       </c>
     </row>
     <row r="24">
@@ -1109,12 +1385,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1539ddc4-5241-5e9d-9086-cc8aea7dcbb1</t>
+          <t>6156d6e1-5c40-5ed7-9144-6856fbfbb067</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Augusto Nunes</t>
+          <t>Andreia Peixoto</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1123,13 +1399,25 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>4963.54282637831</v>
+        <v>8029.53768092652</v>
       </c>
       <c r="F24" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G24" t="n">
-        <v>5053.54282637831</v>
+        <v>90</v>
+      </c>
+      <c r="H24" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I24" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J24" t="n">
+        <v>150</v>
+      </c>
+      <c r="K24" t="n">
+        <v>9153.117680926518</v>
       </c>
     </row>
     <row r="25">
@@ -1138,27 +1426,39 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>361c4b67-5ca5-59d1-998e-08ceca3ebc57</t>
+          <t>61a920cf-a29d-5536-a8ab-3f23dcee4a4b</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bárbara Neves</t>
+          <t>Eliane Jurema</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>4587.767886848967</v>
+        <v>4055.50889721234</v>
       </c>
       <c r="F25" t="n">
-        <v>117</v>
+        <v>533.99</v>
       </c>
       <c r="G25" t="n">
-        <v>4704.767886848967</v>
+        <v>90</v>
+      </c>
+      <c r="H25" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I25" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J25" t="n">
+        <v>50</v>
+      </c>
+      <c r="K25" t="n">
+        <v>5281.25889721234</v>
       </c>
     </row>
     <row r="26">
@@ -1167,12 +1467,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>b2c05943-feee-5add-9b8e-6bdded9a80a9</t>
+          <t>631aa093-f502-5229-8a89-b7392dcec06c</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Beatriz Siqueira</t>
+          <t>André da Rosa</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1181,13 +1481,25 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3230.18657849905</v>
+        <v>7487.999892436921</v>
       </c>
       <c r="F26" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G26" t="n">
-        <v>3320.18657849905</v>
+        <v>90</v>
+      </c>
+      <c r="H26" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I26" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J26" t="n">
+        <v>150</v>
+      </c>
+      <c r="K26" t="n">
+        <v>8700.579892436919</v>
       </c>
     </row>
     <row r="27">
@@ -1196,27 +1508,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>607d85fb-c6b1-57ad-8bbe-b1a93fa57349</t>
+          <t>64bccc6b-6f6b-5e1b-865c-149190776323</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Benedito Silveira</t>
+          <t>Caio Arruda</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1362.231969577253</v>
+        <v>8187.839600815882</v>
       </c>
       <c r="F27" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G27" t="n">
-        <v>1452.231969577253</v>
+        <v>246</v>
+      </c>
+      <c r="H27" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I27" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="n">
+        <v>9350.35960081588</v>
       </c>
     </row>
     <row r="28">
@@ -1225,12 +1547,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>acd778d2-b543-51f4-953c-f9e7e12e7437</t>
+          <t>674419e0-a6fb-5220-acf6-f11f76e231c3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Benjamin Queiroz</t>
+          <t>Bernardo Frota</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1239,13 +1561,25 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>7920.453739691342</v>
+        <v>6387.293051889353</v>
       </c>
       <c r="F28" t="n">
-        <v>206.57</v>
+        <v>364.76</v>
       </c>
       <c r="G28" t="n">
-        <v>8127.023739691342</v>
+        <v>90</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J28" t="n">
+        <v>150</v>
+      </c>
+      <c r="K28" t="n">
+        <v>7289.183051889353</v>
       </c>
     </row>
     <row r="29">
@@ -1254,27 +1588,39 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>674419e0-a6fb-5220-acf6-f11f76e231c3</t>
+          <t>69b08616-ccd0-5227-b382-8bb0265f456f</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bernardo Frota</t>
+          <t>Cláudio Dutra</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>6387.293051889353</v>
+        <v>3997.081814681696</v>
       </c>
       <c r="F29" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G29" t="n">
-        <v>6477.293051889353</v>
+        <v>90</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J29" t="n">
+        <v>10</v>
+      </c>
+      <c r="K29" t="n">
+        <v>4839.201814681695</v>
       </c>
     </row>
     <row r="30">
@@ -1283,12 +1629,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>b60d0f65-4360-5bc9-b58b-4056c9de1119</t>
+          <t>71019c83-dffc-5bad-8c7f-bd61b699add5</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bianca Saraiva</t>
+          <t>Arthur Gusmão</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1297,13 +1643,25 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>6015.101383248207</v>
+        <v>5288.260196934793</v>
       </c>
       <c r="F30" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G30" t="n">
-        <v>6105.101383248207</v>
+        <v>90</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J30" t="n">
+        <v>150</v>
+      </c>
+      <c r="K30" t="n">
+        <v>6270.380196934793</v>
       </c>
     </row>
     <row r="31">
@@ -1312,12 +1670,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>b9f4ce97-2bdc-5c19-8c35-5db4419b4948</t>
+          <t>7339364e-8890-571d-86f0-ddf62dd4b918</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bruna Padilha</t>
+          <t>Douglas Sardinha</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1326,13 +1684,25 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>7266.55679736717</v>
+        <v>2741.365342728207</v>
       </c>
       <c r="F31" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G31" t="n">
-        <v>7356.55679736717</v>
+        <v>90</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J31" t="n">
+        <v>50</v>
+      </c>
+      <c r="K31" t="n">
+        <v>3623.485342728207</v>
       </c>
     </row>
     <row r="32">
@@ -1341,12 +1711,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2f144455-ef5b-5852-8ccb-71bbb361384b</t>
+          <t>73f85436-2fc0-5fc4-840f-f9f03c4fc92b</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bruno Castro</t>
+          <t>Aline da Rocha</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1355,13 +1725,25 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>4610.394047610112</v>
+        <v>1315.118209620667</v>
       </c>
       <c r="F32" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G32" t="n">
-        <v>4700.394047610112</v>
+        <v>90</v>
+      </c>
+      <c r="H32" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I32" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J32" t="n">
+        <v>150</v>
+      </c>
+      <c r="K32" t="n">
+        <v>2551.868209620667</v>
       </c>
     </row>
     <row r="33">
@@ -1370,27 +1752,39 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>64bccc6b-6f6b-5e1b-865c-149190776323</t>
+          <t>7b411419-a6bd-5dac-9123-81532f74e720</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Caio Arruda</t>
+          <t>Elaine Assis</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>8187.839600815882</v>
+        <v>5960.861253655476</v>
       </c>
       <c r="F33" t="n">
-        <v>246</v>
+        <v>533.99</v>
       </c>
       <c r="G33" t="n">
-        <v>8433.839600815882</v>
+        <v>90</v>
+      </c>
+      <c r="H33" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I33" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J33" t="n">
+        <v>50</v>
+      </c>
+      <c r="K33" t="n">
+        <v>7186.611253655476</v>
       </c>
     </row>
     <row r="34">
@@ -1399,12 +1793,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2bc2241b-333d-5e89-9b7c-7c6524872c01</t>
+          <t>95042a82-a9a8-552e-98e3-ac15d20bbf2b</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Camila Dantas</t>
+          <t>Diogo Quintela</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1413,13 +1807,25 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1280.596453813949</v>
+        <v>1461.243910515265</v>
       </c>
       <c r="F34" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G34" t="n">
-        <v>1370.596453813949</v>
+        <v>90</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J34" t="n">
+        <v>50</v>
+      </c>
+      <c r="K34" t="n">
+        <v>2343.363910515265</v>
       </c>
     </row>
     <row r="35">
@@ -1428,27 +1834,39 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>52f4cadd-4009-5089-b7fa-65f6e4ab2887</t>
+          <t>9ae38b1f-abda-5532-a959-7bfada0e0783</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Carlos Magalhães</t>
+          <t>Daniela Drummond</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>8837.775201541868</v>
+        <v>7065.151216079629</v>
       </c>
       <c r="F35" t="n">
-        <v>90</v>
+        <v>684.63</v>
       </c>
       <c r="G35" t="n">
-        <v>8927.775201541868</v>
+        <v>90</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J35" t="n">
+        <v>10</v>
+      </c>
+      <c r="K35" t="n">
+        <v>8146.911216079629</v>
       </c>
     </row>
     <row r="36">
@@ -1457,12 +1875,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>25f4b46b-119b-54b7-a5fa-03827e5ed16f</t>
+          <t>a0b91621-d2a8-537b-95c4-7ade4c6200ee</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Carolina Salgado</t>
+          <t>Edson Furtado</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1471,13 +1889,25 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3266.657357480083</v>
+        <v>7336.902571199591</v>
       </c>
       <c r="F36" t="n">
-        <v>164</v>
+        <v>364.76</v>
       </c>
       <c r="G36" t="n">
-        <v>3430.657357480083</v>
+        <v>90</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J36" t="n">
+        <v>50</v>
+      </c>
+      <c r="K36" t="n">
+        <v>8138.792571199591</v>
       </c>
     </row>
     <row r="37">
@@ -1486,12 +1916,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>b298aa3c-d71a-5df0-83c6-312882b5306b</t>
+          <t>a4b3dbb1-86f1-5d25-95a4-82a6c3076da1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cássia Tavares</t>
+          <t>Alberto da Luz</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1500,13 +1930,25 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>8497.845668097971</v>
+        <v>7364.526801321949</v>
       </c>
       <c r="F37" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G37" t="n">
-        <v>8587.845668097971</v>
+        <v>90</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J37" t="n">
+        <v>150</v>
+      </c>
+      <c r="K37" t="n">
+        <v>8346.646801321949</v>
       </c>
     </row>
     <row r="38">
@@ -1515,12 +1957,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>0eab9fc6-2c73-5288-af73-b13876c87b62</t>
+          <t>acd778d2-b543-51f4-953c-f9e7e12e7437</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Catarina Chaves</t>
+          <t>Benjamin Queiroz</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1529,13 +1971,25 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3490.64446620121</v>
+        <v>7920.453739691342</v>
       </c>
       <c r="F38" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G38" t="n">
-        <v>3580.64446620121</v>
+        <v>206.57</v>
+      </c>
+      <c r="H38" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I38" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J38" t="n">
+        <v>150</v>
+      </c>
+      <c r="K38" t="n">
+        <v>9080.37373969134</v>
       </c>
     </row>
     <row r="39">
@@ -1544,27 +1998,39 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>f35e17a9-38ba-5aa7-9a45-c67338c73cc5</t>
+          <t>b1f0b647-06ea-5aaf-9ea0-a84b2b92563f</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Célia Lemos</t>
+          <t>Edite Marinho</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1212.167158944151</v>
+        <v>800.1804264146962</v>
       </c>
       <c r="F39" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G39" t="n">
-        <v>1302.167158944151</v>
+        <v>90</v>
+      </c>
+      <c r="H39" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I39" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J39" t="n">
+        <v>50</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1856.700426414696</v>
       </c>
     </row>
     <row r="40">
@@ -1573,27 +2039,39 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3d13f1ba-db27-5fa6-9587-1c539c366638</t>
+          <t>b298aa3c-d71a-5df0-83c6-312882b5306b</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Celso Mourão</t>
+          <t>Cássia Tavares</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>257.9421561647101</v>
+        <v>8497.845668097971</v>
       </c>
       <c r="F40" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G40" t="n">
-        <v>347.9421561647101</v>
+        <v>90</v>
+      </c>
+      <c r="H40" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I40" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J40" t="n">
+        <v>10</v>
+      </c>
+      <c r="K40" t="n">
+        <v>9401.195668097969</v>
       </c>
     </row>
     <row r="41">
@@ -1602,12 +2080,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>c57f15e1-0b4a-5ab2-88c8-246678ff4adf</t>
+          <t>b2c05943-feee-5add-9b8e-6bdded9a80a9</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>César Franco</t>
+          <t>Beatriz Siqueira</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1616,13 +2094,25 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>5902.434171124831</v>
+        <v>3230.18657849905</v>
       </c>
       <c r="F41" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G41" t="n">
-        <v>5992.434171124831</v>
+        <v>90</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J41" t="n">
+        <v>150</v>
+      </c>
+      <c r="K41" t="n">
+        <v>4301.30657849905</v>
       </c>
     </row>
     <row r="42">
@@ -1631,27 +2121,39 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>d3819e03-5293-5a6a-82ec-d09fd49e456a</t>
+          <t>b60d0f65-4360-5bc9-b58b-4056c9de1119</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Clarice Barreto</t>
+          <t>Bianca Saraiva</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>9925.179313508823</v>
+        <v>6015.101383248207</v>
       </c>
       <c r="F42" t="n">
-        <v>732</v>
+        <v>364.76</v>
       </c>
       <c r="G42" t="n">
-        <v>10657.17931350882</v>
+        <v>90</v>
+      </c>
+      <c r="H42" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I42" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J42" t="n">
+        <v>150</v>
+      </c>
+      <c r="K42" t="n">
+        <v>7171.621383248207</v>
       </c>
     </row>
     <row r="43">
@@ -1660,27 +2162,39 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>69b08616-ccd0-5227-b382-8bb0265f456f</t>
+          <t>b79ce13c-6117-58b6-bc9e-06eaab0a22bb</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cláudio Dutra</t>
+          <t>Elias Henriques</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>3997.081814681696</v>
+        <v>7306.398876912478</v>
       </c>
       <c r="F43" t="n">
-        <v>90</v>
+        <v>-17.8</v>
       </c>
       <c r="G43" t="n">
-        <v>4087.081814681696</v>
+        <v>90</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J43" t="n">
+        <v>50</v>
+      </c>
+      <c r="K43" t="n">
+        <v>7725.728876912478</v>
       </c>
     </row>
     <row r="44">
@@ -1689,12 +2203,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>f98cdcb6-f68d-5086-b480-7490f8a1675f</t>
+          <t>b96b9339-e1b9-5d20-b70d-67a8bdb16875</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cristiano Vasconcelos</t>
+          <t>Alan Esteves</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1703,13 +2217,25 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>5244.95395791246</v>
+        <v>8059.789738823023</v>
       </c>
       <c r="F44" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G44" t="n">
-        <v>5334.95395791246</v>
+        <v>90</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J44" t="n">
+        <v>150</v>
+      </c>
+      <c r="K44" t="n">
+        <v>9041.909738823022</v>
       </c>
     </row>
     <row r="45">
@@ -1718,27 +2244,37 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3f4a1eeb-c287-57d9-8407-78ea76ba96ea</t>
+          <t>b9f4ce97-2bdc-5c19-8c35-5db4419b4948</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cristina Meireles</t>
+          <t>Bruna Padilha</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>6183.77422031294</v>
+        <v>7266.55679736717</v>
       </c>
       <c r="F45" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G45" t="n">
-        <v>6273.77422031294</v>
+        <v>90</v>
+      </c>
+      <c r="H45" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I45" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="n">
+        <v>8442.30679736717</v>
       </c>
     </row>
     <row r="46">
@@ -1747,27 +2283,39 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>da7b82a2-d4bc-5993-8e5f-59aa3081241a</t>
+          <t>c4998a9b-cc38-5851-9223-7cf43ea91c36</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Daniel Bezerra</t>
+          <t>Alice Farias</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>6173.403303137569</v>
+        <v>8284.136836853117</v>
       </c>
       <c r="F46" t="n">
-        <v>90</v>
+        <v>560.7</v>
       </c>
       <c r="G46" t="n">
-        <v>6263.403303137569</v>
+        <v>90</v>
+      </c>
+      <c r="H46" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I46" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J46" t="n">
+        <v>150</v>
+      </c>
+      <c r="K46" t="n">
+        <v>9636.596836853116</v>
       </c>
     </row>
     <row r="47">
@@ -1776,27 +2324,39 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9ae38b1f-abda-5532-a959-7bfada0e0783</t>
+          <t>c4fd9f54-9504-52b3-9fca-ab39c50dc07f</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Daniela Drummond</t>
+          <t>Anselmo Novaes</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>7065.151216079629</v>
+        <v>1108.340345861018</v>
       </c>
       <c r="F47" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G47" t="n">
-        <v>7155.151216079629</v>
+        <v>90</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J47" t="n">
+        <v>150</v>
+      </c>
+      <c r="K47" t="n">
+        <v>2090.460345861018</v>
       </c>
     </row>
     <row r="48">
@@ -1805,12 +2365,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06be0738-b15f-5d07-892b-d45971647c79</t>
+          <t>c57f15e1-0b4a-5ab2-88c8-246678ff4adf</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Danilo Brandão</t>
+          <t>César Franco</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1819,13 +2379,25 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>9095.090151715545</v>
+        <v>5902.434171124831</v>
       </c>
       <c r="F48" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>9185.090151715545</v>
+        <v>90</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J48" t="n">
+        <v>10</v>
+      </c>
+      <c r="K48" t="n">
+        <v>6299.564171124831</v>
       </c>
     </row>
     <row r="49">
@@ -1834,27 +2406,37 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ec7d2162-5de8-50e9-9aea-a1dd90ec8081</t>
+          <t>c8fdc760-5724-5f8c-82ae-2e6e767b3811</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Davi Caldeira</t>
+          <t>Denis Macedo</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>746.9510783679258</v>
+        <v>3952.204962932551</v>
       </c>
       <c r="F49" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G49" t="n">
-        <v>836.9510783679258</v>
+        <v>164</v>
+      </c>
+      <c r="H49" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I49" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="n">
+        <v>5032.724962932551</v>
       </c>
     </row>
     <row r="50">
@@ -1863,27 +2445,39 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ca78df0b-cb88-5905-ab6f-c47150af2c20</t>
+          <t>ca2f5a2d-c388-5837-ae1f-93173331ba9a</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Débora Guedes</t>
+          <t>Alexandre da Mata</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>8733.661290965678</v>
+        <v>9551.21905794158</v>
       </c>
       <c r="F50" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G50" t="n">
-        <v>8823.661290965678</v>
+        <v>90</v>
+      </c>
+      <c r="H50" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I50" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J50" t="n">
+        <v>150</v>
+      </c>
+      <c r="K50" t="n">
+        <v>10707.73905794158</v>
       </c>
     </row>
     <row r="51">
@@ -1892,27 +2486,39 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>c8fdc760-5724-5f8c-82ae-2e6e767b3811</t>
+          <t>ca78df0b-cb88-5905-ab6f-c47150af2c20</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Denis Macedo</t>
+          <t>Débora Guedes</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3952.204962932551</v>
+        <v>8733.661290965678</v>
       </c>
       <c r="F51" t="n">
-        <v>164</v>
+        <v>855.8</v>
       </c>
       <c r="G51" t="n">
-        <v>4116.20496293255</v>
+        <v>90</v>
+      </c>
+      <c r="H51" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I51" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J51" t="n">
+        <v>10</v>
+      </c>
+      <c r="K51" t="n">
+        <v>10241.22129096568</v>
       </c>
     </row>
     <row r="52">
@@ -1921,12 +2527,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>17533122-8361-509c-9e67-8887db2e0001</t>
+          <t>ce6652c4-e8d1-5805-81c2-2fdc603f51b0</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Diana Azevedo</t>
+          <t>Antônio Viana</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1935,13 +2541,25 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>6993.13850131002</v>
+        <v>3295.032751492262</v>
       </c>
       <c r="F52" t="n">
-        <v>90</v>
+        <v>560.7</v>
       </c>
       <c r="G52" t="n">
-        <v>7083.13850131002</v>
+        <v>117</v>
+      </c>
+      <c r="H52" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I52" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J52" t="n">
+        <v>150</v>
+      </c>
+      <c r="K52" t="n">
+        <v>4674.492751492262</v>
       </c>
     </row>
     <row r="53">
@@ -1950,27 +2568,39 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4b86c62c-6ddf-539d-ac69-cc6cc522386a</t>
+          <t>d3819e03-5293-5a6a-82ec-d09fd49e456a</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Diego Figueiredo</t>
+          <t>Clarice Barreto</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>490.174359132607</v>
+        <v>9925.179313508823</v>
       </c>
       <c r="F53" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G53" t="n">
-        <v>580.1743591326069</v>
+        <v>732</v>
+      </c>
+      <c r="H53" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I53" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J53" t="n">
+        <v>10</v>
+      </c>
+      <c r="K53" t="n">
+        <v>11583.69931350882</v>
       </c>
     </row>
     <row r="54">
@@ -1979,12 +2609,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>95042a82-a9a8-552e-98e3-ac15d20bbf2b</t>
+          <t>d4d9f427-c9cd-5935-a88d-60bb469e7c89</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Diogo Quintela</t>
+          <t>Álvaro da Paz</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1993,13 +2623,25 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1461.243910515265</v>
+        <v>1223.312552727439</v>
       </c>
       <c r="F54" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G54" t="n">
-        <v>1551.243910515265</v>
+        <v>90</v>
+      </c>
+      <c r="H54" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I54" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J54" t="n">
+        <v>150</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2549.062552727439</v>
       </c>
     </row>
     <row r="55">
@@ -2008,27 +2650,39 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7339364e-8890-571d-86f0-ddf62dd4b918</t>
+          <t>d5426380-369f-500b-a136-ce5543c13c0d</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Douglas Sardinha</t>
+          <t>Edgar Cordeiro</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>2741.365342728207</v>
+        <v>4455.059040524839</v>
       </c>
       <c r="F55" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G55" t="n">
-        <v>2831.365342728207</v>
+        <v>90</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J55" t="n">
+        <v>50</v>
+      </c>
+      <c r="K55" t="n">
+        <v>5337.179040524838</v>
       </c>
     </row>
     <row r="56">
@@ -2037,12 +2691,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>d5426380-369f-500b-a136-ce5543c13c0d</t>
+          <t>da7b82a2-d4bc-5993-8e5f-59aa3081241a</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Edgar Cordeiro</t>
+          <t>Daniel Bezerra</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2051,13 +2705,25 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>4455.059040524839</v>
+        <v>6173.403303137569</v>
       </c>
       <c r="F56" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G56" t="n">
-        <v>4545.059040524839</v>
+        <v>90</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J56" t="n">
+        <v>10</v>
+      </c>
+      <c r="K56" t="n">
+        <v>7015.523303137569</v>
       </c>
     </row>
     <row r="57">
@@ -2066,27 +2732,37 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>b1f0b647-06ea-5aaf-9ea0-a84b2b92563f</t>
+          <t>db0b9e18-aa43-5a04-b686-ac454728ad3a</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Edite Marinho</t>
+          <t>Elielson Quadros</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>800.1804264146962</v>
+        <v>6715.641722399166</v>
       </c>
       <c r="F57" t="n">
-        <v>90</v>
+        <v>498.39</v>
       </c>
       <c r="G57" t="n">
-        <v>890.1804264146962</v>
+        <v>90</v>
+      </c>
+      <c r="H57" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I57" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="n">
+        <v>7855.791722399166</v>
       </c>
     </row>
     <row r="58">
@@ -2095,12 +2771,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>a0b91621-d2a8-537b-95c4-7ade4c6200ee</t>
+          <t>ea3147dc-902e-5ded-88e8-10514c53e142</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Edson Furtado</t>
+          <t>Ana Melo</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2109,13 +2785,25 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>7336.902571199591</v>
+        <v>8057.257421621038</v>
       </c>
       <c r="F58" t="n">
-        <v>90</v>
+        <v>444.99</v>
       </c>
       <c r="G58" t="n">
-        <v>7426.902571199591</v>
+        <v>90</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J58" t="n">
+        <v>150</v>
+      </c>
+      <c r="K58" t="n">
+        <v>9039.377421621037</v>
       </c>
     </row>
     <row r="59">
@@ -2124,12 +2812,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2c297031-afd1-540c-a226-32291c3b420d</t>
+          <t>ec7d2162-5de8-50e9-9aea-a1dd90ec8081</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Eduardo Portela</t>
+          <t>Davi Caldeira</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2138,13 +2826,25 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1728.629771639805</v>
+        <v>746.9510783679258</v>
       </c>
       <c r="F59" t="n">
-        <v>117</v>
+        <v>560.7</v>
       </c>
       <c r="G59" t="n">
-        <v>1845.629771639805</v>
+        <v>90</v>
+      </c>
+      <c r="H59" t="n">
+        <v>254.63</v>
+      </c>
+      <c r="I59" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J59" t="n">
+        <v>10</v>
+      </c>
+      <c r="K59" t="n">
+        <v>1959.411078367926</v>
       </c>
     </row>
     <row r="60">
@@ -2153,27 +2853,39 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7b411419-a6bd-5dac-9123-81532f74e720</t>
+          <t>f08290a7-3372-5637-9244-a80f8bc9ee3c</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Elaine Assis</t>
+          <t>Ângela Rezende</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>5960.861253655476</v>
+        <v>2036.514997025348</v>
       </c>
       <c r="F60" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G60" t="n">
-        <v>6050.861253655476</v>
+        <v>90</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J60" t="n">
+        <v>150</v>
+      </c>
+      <c r="K60" t="n">
+        <v>2938.404997025348</v>
       </c>
     </row>
     <row r="61">
@@ -2182,12 +2894,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>b79ce13c-6117-58b6-bc9e-06eaab0a22bb</t>
+          <t>f35e17a9-38ba-5aa7-9a45-c67338c73cc5</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Elias Henriques</t>
+          <t>Célia Lemos</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2196,13 +2908,25 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>7306.398876912478</v>
+        <v>1212.167158944151</v>
       </c>
       <c r="F61" t="n">
-        <v>90</v>
+        <v>364.76</v>
       </c>
       <c r="G61" t="n">
-        <v>7396.398876912478</v>
+        <v>90</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J61" t="n">
+        <v>10</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1974.057158944151</v>
       </c>
     </row>
     <row r="62">
@@ -2211,27 +2935,39 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>61a920cf-a29d-5536-a8ab-3f23dcee4a4b</t>
+          <t>f98cdcb6-f68d-5086-b480-7490f8a1675f</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Eliane Jurema</t>
+          <t>Cristiano Vasconcelos</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>4055.50889721234</v>
+        <v>5244.95395791246</v>
       </c>
       <c r="F62" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G62" t="n">
-        <v>4145.508897212339</v>
+        <v>90</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J62" t="n">
+        <v>10</v>
+      </c>
+      <c r="K62" t="n">
+        <v>6176.07395791246</v>
       </c>
     </row>
     <row r="63">
@@ -2240,27 +2976,58 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>db0b9e18-aa43-5a04-b686-ac454728ad3a</t>
+          <t>f9e02392-bc91-5868-91d5-4a90ccc2cbbf</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Elielson Quadros</t>
+          <t>Anderson Aragão</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>6715.641722399166</v>
+        <v>9712.728285382607</v>
       </c>
       <c r="F63" t="n">
-        <v>90</v>
+        <v>533.99</v>
       </c>
       <c r="G63" t="n">
-        <v>6805.641722399166</v>
+        <v>90</v>
+      </c>
+      <c r="H63" t="n">
+        <v>141.46</v>
+      </c>
+      <c r="I63" t="n">
+        <v>297.13</v>
+      </c>
+      <c r="J63" t="n">
+        <v>150</v>
+      </c>
+      <c r="K63" t="n">
+        <v>10925.30828538261</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="n">
+        <v>50</v>
+      </c>
+      <c r="K64" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(exec_func): fix sum columns and dataframe copy
- fix sum columns to absolute values
- fix final dataframe to get the last one
</commit_message>
<xml_diff>
--- a/output/custos_por_colaborador.xlsx
+++ b/output/custos_por_colaborador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,11 +476,6 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Custo Claude</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
           <t>Custo Total</t>
         </is>
       </c>
@@ -491,12 +486,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>00a0d290-74eb-5793-8df7-98f4280eb295</t>
+          <t>177d2a03-dd33-5953-8650-1de95414461f</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Antônia Pires</t>
+          <t>Adolfo Moreira</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -505,10 +500,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>9976.53102463056</v>
+        <v>3384.960765580439</v>
       </c>
       <c r="F2" t="n">
-        <v>444.99</v>
+        <v>533.99</v>
       </c>
       <c r="G2" t="n">
         <v>90</v>
@@ -520,10 +515,7 @@
         <v>297.13</v>
       </c>
       <c r="J2" t="n">
-        <v>150</v>
-      </c>
-      <c r="K2" t="n">
-        <v>11213.28102463056</v>
+        <v>4560.710765580439</v>
       </c>
     </row>
     <row r="3">
@@ -532,12 +524,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>06be0738-b15f-5d07-892b-d45971647c79</t>
+          <t>41cf3515-ef53-595d-a1e6-4d127d75533b</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Danilo Brandão</t>
+          <t>Adriana Nogueira</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -546,7 +538,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>9095.090151715545</v>
+        <v>3719.103451680459</v>
       </c>
       <c r="F3" t="n">
         <v>855.8</v>
@@ -561,10 +553,7 @@
         <v>297.13</v>
       </c>
       <c r="J3" t="n">
-        <v>10</v>
-      </c>
-      <c r="K3" t="n">
-        <v>10348.02015171554</v>
+        <v>4962.033451680459</v>
       </c>
     </row>
     <row r="4">
@@ -573,21 +562,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0eab9fc6-2c73-5288-af73-b13876c87b62</t>
+          <t>39f92dc0-2ae9-596f-a160-35025eebbff1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Catarina Chaves</t>
+          <t>Afonso Barros</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3490.64446620121</v>
+        <v>8962.729721841501</v>
       </c>
       <c r="F4" t="n">
         <v>444.99</v>
@@ -596,16 +585,13 @@
         <v>90</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>141.46</v>
       </c>
       <c r="I4" t="n">
         <v>297.13</v>
       </c>
       <c r="J4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K4" t="n">
-        <v>4332.76446620121</v>
+        <v>9936.309721841499</v>
       </c>
     </row>
     <row r="5">
@@ -614,39 +600,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1202a201-05dd-5f81-bff7-762f946c273e</t>
+          <t>b96b9339-e1b9-5d20-b70d-67a8bdb16875</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ariane Teixeira</t>
+          <t>Alan Esteves</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>8271.84079484528</v>
+        <v>8059.789738823023</v>
       </c>
       <c r="F5" t="n">
-        <v>533.99</v>
+        <v>444.99</v>
       </c>
       <c r="G5" t="n">
         <v>90</v>
       </c>
       <c r="H5" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>297.13</v>
       </c>
       <c r="J5" t="n">
-        <v>150</v>
-      </c>
-      <c r="K5" t="n">
-        <v>9597.590794845279</v>
+        <v>8891.909738823022</v>
       </c>
     </row>
     <row r="6">
@@ -655,12 +638,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1539ddc4-5241-5e9d-9086-cc8aea7dcbb1</t>
+          <t>a4b3dbb1-86f1-5d25-95a4-82a6c3076da1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Augusto Nunes</t>
+          <t>Alberto da Luz</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -669,25 +652,22 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4963.54282637831</v>
+        <v>7364.526801321949</v>
       </c>
       <c r="F6" t="n">
-        <v>560.7</v>
+        <v>444.99</v>
       </c>
       <c r="G6" t="n">
         <v>90</v>
       </c>
       <c r="H6" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>297.13</v>
       </c>
       <c r="J6" t="n">
-        <v>150</v>
-      </c>
-      <c r="K6" t="n">
-        <v>6316.00282637831</v>
+        <v>8196.646801321949</v>
       </c>
     </row>
     <row r="7">
@@ -696,12 +676,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17533122-8361-509c-9e67-8887db2e0001</t>
+          <t>282b242b-4e87-51f2-a5ff-d141bd8825c8</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Diana Azevedo</t>
+          <t>Alessandra Dias</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -710,10 +690,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6993.13850131002</v>
+        <v>5318.987724937523</v>
       </c>
       <c r="F7" t="n">
-        <v>-328.28</v>
+        <v>444.99</v>
       </c>
       <c r="G7" t="n">
         <v>90</v>
@@ -724,9 +704,8 @@
       <c r="I7" t="n">
         <v>297.13</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="n">
-        <v>7051.98850131002</v>
+      <c r="J7" t="n">
+        <v>6151.107724937523</v>
       </c>
     </row>
     <row r="8">
@@ -735,12 +714,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>177d2a03-dd33-5953-8650-1de95414461f</t>
+          <t>ca2f5a2d-c388-5837-ae1f-93173331ba9a</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Adolfo Moreira</t>
+          <t>Alexandre da Mata</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -749,10 +728,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3384.960765580439</v>
+        <v>9551.21905794158</v>
       </c>
       <c r="F8" t="n">
-        <v>533.99</v>
+        <v>364.76</v>
       </c>
       <c r="G8" t="n">
         <v>90</v>
@@ -764,10 +743,7 @@
         <v>297.13</v>
       </c>
       <c r="J8" t="n">
-        <v>150</v>
-      </c>
-      <c r="K8" t="n">
-        <v>4710.710765580439</v>
+        <v>10557.73905794158</v>
       </c>
     </row>
     <row r="9">
@@ -776,39 +752,36 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>25f4b46b-119b-54b7-a5fa-03827e5ed16f</t>
+          <t>c4998a9b-cc38-5851-9223-7cf43ea91c36</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Carolina Salgado</t>
+          <t>Alice Farias</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3266.657357480083</v>
+        <v>8284.136836853117</v>
       </c>
       <c r="F9" t="n">
-        <v>364.76</v>
+        <v>560.7</v>
       </c>
       <c r="G9" t="n">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I9" t="n">
         <v>297.13</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
-      </c>
-      <c r="K9" t="n">
-        <v>4102.547357480083</v>
+        <v>9486.596836853116</v>
       </c>
     </row>
     <row r="10">
@@ -817,12 +790,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>282b242b-4e87-51f2-a5ff-d141bd8825c8</t>
+          <t>73f85436-2fc0-5fc4-840f-f9f03c4fc92b</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Alessandra Dias</t>
+          <t>Aline da Rocha</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -831,7 +804,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>5318.987724937523</v>
+        <v>1315.118209620667</v>
       </c>
       <c r="F10" t="n">
         <v>444.99</v>
@@ -840,16 +813,13 @@
         <v>90</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I10" t="n">
         <v>297.13</v>
       </c>
       <c r="J10" t="n">
-        <v>150</v>
-      </c>
-      <c r="K10" t="n">
-        <v>6301.107724937523</v>
+        <v>2401.868209620667</v>
       </c>
     </row>
     <row r="11">
@@ -858,12 +828,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2bc2241b-333d-5e89-9b7c-7c6524872c01</t>
+          <t>d4d9f427-c9cd-5935-a88d-60bb469e7c89</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Camila Dantas</t>
+          <t>Álvaro da Paz</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -872,10 +842,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1280.596453813949</v>
+        <v>1223.312552727439</v>
       </c>
       <c r="F11" t="n">
-        <v>444.99</v>
+        <v>533.99</v>
       </c>
       <c r="G11" t="n">
         <v>90</v>
@@ -886,9 +856,8 @@
       <c r="I11" t="n">
         <v>297.13</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="n">
-        <v>2367.346453813949</v>
+      <c r="J11" t="n">
+        <v>2399.062552727439</v>
       </c>
     </row>
     <row r="12">
@@ -897,12 +866,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2c297031-afd1-540c-a226-32291c3b420d</t>
+          <t>442868a8-fabc-5568-a849-51f72b08b3c7</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Eduardo Portela</t>
+          <t>Amanda Pinto</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -911,13 +880,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1728.629771639805</v>
+        <v>4021.833629163991</v>
       </c>
       <c r="F12" t="n">
-        <v>560.7</v>
+        <v>848.05</v>
       </c>
       <c r="G12" t="n">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -926,10 +895,7 @@
         <v>297.13</v>
       </c>
       <c r="J12" t="n">
-        <v>50</v>
-      </c>
-      <c r="K12" t="n">
-        <v>2753.459771639805</v>
+        <v>5257.013629163991</v>
       </c>
     </row>
     <row r="13">
@@ -938,12 +904,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2f144455-ef5b-5852-8ccb-71bbb361384b</t>
+          <t>56f44ead-fafa-5e60-a0a7-e51d81a79de8</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bruno Castro</t>
+          <t>Amélia Ribeiro</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -952,23 +918,22 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4610.394047610112</v>
+        <v>5244.623025188975</v>
       </c>
       <c r="F13" t="n">
-        <v>364.76</v>
+        <v>533.99</v>
       </c>
       <c r="G13" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="H13" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>297.13</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="n">
-        <v>5616.914047610113</v>
+      <c r="J13" t="n">
+        <v>6192.743025188975</v>
       </c>
     </row>
     <row r="14">
@@ -977,12 +942,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>361c4b67-5ca5-59d1-998e-08ceca3ebc57</t>
+          <t>ea3147dc-902e-5ded-88e8-10514c53e142</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bárbara Neves</t>
+          <t>Ana Melo</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -991,13 +956,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4587.767886848967</v>
+        <v>8057.257421621038</v>
       </c>
       <c r="F14" t="n">
-        <v>364.76</v>
+        <v>444.99</v>
       </c>
       <c r="G14" t="n">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1006,10 +971,7 @@
         <v>297.13</v>
       </c>
       <c r="J14" t="n">
-        <v>150</v>
-      </c>
-      <c r="K14" t="n">
-        <v>5516.657886848967</v>
+        <v>8889.377421621037</v>
       </c>
     </row>
     <row r="15">
@@ -1018,12 +980,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>39f92dc0-2ae9-596f-a160-35025eebbff1</t>
+          <t>f9e02392-bc91-5868-91d5-4a90ccc2cbbf</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Afonso Barros</t>
+          <t>Anderson Aragão</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1032,10 +994,10 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>8962.729721841501</v>
+        <v>9712.728285382607</v>
       </c>
       <c r="F15" t="n">
-        <v>444.99</v>
+        <v>533.99</v>
       </c>
       <c r="G15" t="n">
         <v>90</v>
@@ -1047,10 +1009,7 @@
         <v>297.13</v>
       </c>
       <c r="J15" t="n">
-        <v>150</v>
-      </c>
-      <c r="K15" t="n">
-        <v>10086.3097218415</v>
+        <v>10775.30828538261</v>
       </c>
     </row>
     <row r="16">
@@ -1059,39 +1018,36 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3d13f1ba-db27-5fa6-9587-1c539c366638</t>
+          <t>631aa093-f502-5229-8a89-b7392dcec06c</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Celso Mourão</t>
+          <t>André da Rosa</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>257.9421561647101</v>
+        <v>7487.999892436921</v>
       </c>
       <c r="F16" t="n">
-        <v>404.91</v>
+        <v>533.99</v>
       </c>
       <c r="G16" t="n">
         <v>90</v>
       </c>
       <c r="H16" t="n">
-        <v>254.63</v>
+        <v>141.46</v>
       </c>
       <c r="I16" t="n">
         <v>297.13</v>
       </c>
       <c r="J16" t="n">
-        <v>10</v>
-      </c>
-      <c r="K16" t="n">
-        <v>1314.61215616471</v>
+        <v>8550.579892436919</v>
       </c>
     </row>
     <row r="17">
@@ -1100,12 +1056,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3f4a1eeb-c287-57d9-8407-78ea76ba96ea</t>
+          <t>6156d6e1-5c40-5ed7-9144-6856fbfbb067</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Cristina Meireles</t>
+          <t>Andreia Peixoto</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1114,25 +1070,22 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>6183.77422031294</v>
+        <v>8029.53768092652</v>
       </c>
       <c r="F17" t="n">
-        <v>364.76</v>
+        <v>444.99</v>
       </c>
       <c r="G17" t="n">
         <v>90</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>141.46</v>
       </c>
       <c r="I17" t="n">
         <v>297.13</v>
       </c>
       <c r="J17" t="n">
-        <v>10</v>
-      </c>
-      <c r="K17" t="n">
-        <v>6945.66422031294</v>
+        <v>9003.117680926518</v>
       </c>
     </row>
     <row r="18">
@@ -1141,24 +1094,24 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>41cf3515-ef53-595d-a1e6-4d127d75533b</t>
+          <t>f08290a7-3372-5637-9244-a80f8bc9ee3c</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Adriana Nogueira</t>
+          <t>Ângela Rezende</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3719.103451680459</v>
+        <v>2036.514997025348</v>
       </c>
       <c r="F18" t="n">
-        <v>855.8</v>
+        <v>364.76</v>
       </c>
       <c r="G18" t="n">
         <v>90</v>
@@ -1170,10 +1123,7 @@
         <v>297.13</v>
       </c>
       <c r="J18" t="n">
-        <v>150</v>
-      </c>
-      <c r="K18" t="n">
-        <v>5112.033451680459</v>
+        <v>2788.404997025348</v>
       </c>
     </row>
     <row r="19">
@@ -1182,12 +1132,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>442868a8-fabc-5568-a849-51f72b08b3c7</t>
+          <t>c4fd9f54-9504-52b3-9fca-ab39c50dc07f</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Amanda Pinto</t>
+          <t>Anselmo Novaes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1196,10 +1146,10 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>4021.833629163991</v>
+        <v>1108.340345861018</v>
       </c>
       <c r="F19" t="n">
-        <v>848.05</v>
+        <v>444.99</v>
       </c>
       <c r="G19" t="n">
         <v>90</v>
@@ -1211,10 +1161,7 @@
         <v>297.13</v>
       </c>
       <c r="J19" t="n">
-        <v>150</v>
-      </c>
-      <c r="K19" t="n">
-        <v>5407.013629163991</v>
+        <v>1940.460345861018</v>
       </c>
     </row>
     <row r="20">
@@ -1223,24 +1170,24 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4b86c62c-6ddf-539d-ac69-cc6cc522386a</t>
+          <t>00a0d290-74eb-5793-8df7-98f4280eb295</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Diego Figueiredo</t>
+          <t>Antônia Pires</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>490.174359132607</v>
+        <v>9976.53102463056</v>
       </c>
       <c r="F20" t="n">
-        <v>622.41</v>
+        <v>444.99</v>
       </c>
       <c r="G20" t="n">
         <v>90</v>
@@ -1251,9 +1198,8 @@
       <c r="I20" t="n">
         <v>297.13</v>
       </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="n">
-        <v>1754.344359132607</v>
+      <c r="J20" t="n">
+        <v>11063.28102463056</v>
       </c>
     </row>
     <row r="21">
@@ -1262,12 +1208,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>52f4cadd-4009-5089-b7fa-65f6e4ab2887</t>
+          <t>ce6652c4-e8d1-5805-81c2-2fdc603f51b0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Carlos Magalhães</t>
+          <t>Antônio Viana</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1276,13 +1222,13 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>8837.775201541868</v>
+        <v>3295.032751492262</v>
       </c>
       <c r="F21" t="n">
-        <v>364.76</v>
+        <v>560.7</v>
       </c>
       <c r="G21" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="H21" t="n">
         <v>254.63</v>
@@ -1291,10 +1237,7 @@
         <v>297.13</v>
       </c>
       <c r="J21" t="n">
-        <v>10</v>
-      </c>
-      <c r="K21" t="n">
-        <v>9854.295201541867</v>
+        <v>4524.492751492262</v>
       </c>
     </row>
     <row r="22">
@@ -1303,39 +1246,36 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>56f44ead-fafa-5e60-a0a7-e51d81a79de8</t>
+          <t>1202a201-05dd-5f81-bff7-762f946c273e</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Amélia Ribeiro</t>
+          <t>Ariane Teixeira</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>5244.623025188975</v>
+        <v>8271.84079484528</v>
       </c>
       <c r="F22" t="n">
         <v>533.99</v>
       </c>
       <c r="G22" t="n">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I22" t="n">
         <v>297.13</v>
       </c>
       <c r="J22" t="n">
-        <v>150</v>
-      </c>
-      <c r="K22" t="n">
-        <v>6342.743025188975</v>
+        <v>9447.590794845279</v>
       </c>
     </row>
     <row r="23">
@@ -1344,21 +1284,21 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>607d85fb-c6b1-57ad-8bbe-b1a93fa57349</t>
+          <t>71019c83-dffc-5bad-8c7f-bd61b699add5</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Benedito Silveira</t>
+          <t>Arthur Gusmão</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1362.231969577253</v>
+        <v>5288.260196934793</v>
       </c>
       <c r="F23" t="n">
         <v>444.99</v>
@@ -1373,10 +1313,7 @@
         <v>297.13</v>
       </c>
       <c r="J23" t="n">
-        <v>150</v>
-      </c>
-      <c r="K23" t="n">
-        <v>2344.351969577253</v>
+        <v>6120.380196934793</v>
       </c>
     </row>
     <row r="24">
@@ -1385,12 +1322,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6156d6e1-5c40-5ed7-9144-6856fbfbb067</t>
+          <t>1539ddc4-5241-5e9d-9086-cc8aea7dcbb1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Andreia Peixoto</t>
+          <t>Augusto Nunes</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1399,25 +1336,22 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>8029.53768092652</v>
+        <v>4963.54282637831</v>
       </c>
       <c r="F24" t="n">
-        <v>444.99</v>
+        <v>560.7</v>
       </c>
       <c r="G24" t="n">
         <v>90</v>
       </c>
       <c r="H24" t="n">
-        <v>141.46</v>
+        <v>254.63</v>
       </c>
       <c r="I24" t="n">
         <v>297.13</v>
       </c>
       <c r="J24" t="n">
-        <v>150</v>
-      </c>
-      <c r="K24" t="n">
-        <v>9153.117680926518</v>
+        <v>6166.00282637831</v>
       </c>
     </row>
     <row r="25">
@@ -1426,39 +1360,36 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>61a920cf-a29d-5536-a8ab-3f23dcee4a4b</t>
+          <t>361c4b67-5ca5-59d1-998e-08ceca3ebc57</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Eliane Jurema</t>
+          <t>Bárbara Neves</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>4055.50889721234</v>
+        <v>4587.767886848967</v>
       </c>
       <c r="F25" t="n">
-        <v>533.99</v>
+        <v>364.76</v>
       </c>
       <c r="G25" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="H25" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>297.13</v>
       </c>
       <c r="J25" t="n">
-        <v>50</v>
-      </c>
-      <c r="K25" t="n">
-        <v>5281.25889721234</v>
+        <v>5366.657886848967</v>
       </c>
     </row>
     <row r="26">
@@ -1467,12 +1398,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>631aa093-f502-5229-8a89-b7392dcec06c</t>
+          <t>b2c05943-feee-5add-9b8e-6bdded9a80a9</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>André da Rosa</t>
+          <t>Beatriz Siqueira</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1481,7 +1412,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>7487.999892436921</v>
+        <v>3230.18657849905</v>
       </c>
       <c r="F26" t="n">
         <v>533.99</v>
@@ -1490,16 +1421,13 @@
         <v>90</v>
       </c>
       <c r="H26" t="n">
-        <v>141.46</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
         <v>297.13</v>
       </c>
       <c r="J26" t="n">
-        <v>150</v>
-      </c>
-      <c r="K26" t="n">
-        <v>8700.579892436919</v>
+        <v>4151.30657849905</v>
       </c>
     </row>
     <row r="27">
@@ -1508,37 +1436,36 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>64bccc6b-6f6b-5e1b-865c-149190776323</t>
+          <t>607d85fb-c6b1-57ad-8bbe-b1a93fa57349</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Caio Arruda</t>
+          <t>Benedito Silveira</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>8187.839600815882</v>
+        <v>1362.231969577253</v>
       </c>
       <c r="F27" t="n">
-        <v>364.76</v>
+        <v>444.99</v>
       </c>
       <c r="G27" t="n">
-        <v>246</v>
+        <v>90</v>
       </c>
       <c r="H27" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>297.13</v>
       </c>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="n">
-        <v>9350.35960081588</v>
+      <c r="J27" t="n">
+        <v>2194.351969577253</v>
       </c>
     </row>
     <row r="28">
@@ -1547,12 +1474,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>674419e0-a6fb-5220-acf6-f11f76e231c3</t>
+          <t>acd778d2-b543-51f4-953c-f9e7e12e7437</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bernardo Frota</t>
+          <t>Benjamin Queiroz</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1561,25 +1488,22 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>6387.293051889353</v>
+        <v>7920.453739691342</v>
       </c>
       <c r="F28" t="n">
         <v>364.76</v>
       </c>
       <c r="G28" t="n">
-        <v>90</v>
+        <v>206.57</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>141.46</v>
       </c>
       <c r="I28" t="n">
         <v>297.13</v>
       </c>
       <c r="J28" t="n">
-        <v>150</v>
-      </c>
-      <c r="K28" t="n">
-        <v>7289.183051889353</v>
+        <v>8930.37373969134</v>
       </c>
     </row>
     <row r="29">
@@ -1588,24 +1512,24 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>69b08616-ccd0-5227-b382-8bb0265f456f</t>
+          <t>674419e0-a6fb-5220-acf6-f11f76e231c3</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cláudio Dutra</t>
+          <t>Bernardo Frota</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3997.081814681696</v>
+        <v>6387.293051889353</v>
       </c>
       <c r="F29" t="n">
-        <v>444.99</v>
+        <v>364.76</v>
       </c>
       <c r="G29" t="n">
         <v>90</v>
@@ -1617,10 +1541,7 @@
         <v>297.13</v>
       </c>
       <c r="J29" t="n">
-        <v>10</v>
-      </c>
-      <c r="K29" t="n">
-        <v>4839.201814681695</v>
+        <v>7139.183051889353</v>
       </c>
     </row>
     <row r="30">
@@ -1629,12 +1550,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>71019c83-dffc-5bad-8c7f-bd61b699add5</t>
+          <t>b60d0f65-4360-5bc9-b58b-4056c9de1119</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Arthur Gusmão</t>
+          <t>Bianca Saraiva</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1643,25 +1564,22 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>5288.260196934793</v>
+        <v>6015.101383248207</v>
       </c>
       <c r="F30" t="n">
-        <v>444.99</v>
+        <v>364.76</v>
       </c>
       <c r="G30" t="n">
         <v>90</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I30" t="n">
         <v>297.13</v>
       </c>
       <c r="J30" t="n">
-        <v>150</v>
-      </c>
-      <c r="K30" t="n">
-        <v>6270.380196934793</v>
+        <v>7021.621383248207</v>
       </c>
     </row>
     <row r="31">
@@ -1670,12 +1588,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>7339364e-8890-571d-86f0-ddf62dd4b918</t>
+          <t>b9f4ce97-2bdc-5c19-8c35-5db4419b4948</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Douglas Sardinha</t>
+          <t>Bruna Padilha</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1684,25 +1602,22 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2741.365342728207</v>
+        <v>7266.55679736717</v>
       </c>
       <c r="F31" t="n">
-        <v>444.99</v>
+        <v>533.99</v>
       </c>
       <c r="G31" t="n">
         <v>90</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I31" t="n">
         <v>297.13</v>
       </c>
       <c r="J31" t="n">
-        <v>50</v>
-      </c>
-      <c r="K31" t="n">
-        <v>3623.485342728207</v>
+        <v>8442.30679736717</v>
       </c>
     </row>
     <row r="32">
@@ -1711,12 +1626,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>73f85436-2fc0-5fc4-840f-f9f03c4fc92b</t>
+          <t>2f144455-ef5b-5852-8ccb-71bbb361384b</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Aline da Rocha</t>
+          <t>Bruno Castro</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1725,10 +1640,10 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1315.118209620667</v>
+        <v>4610.394047610112</v>
       </c>
       <c r="F32" t="n">
-        <v>444.99</v>
+        <v>364.76</v>
       </c>
       <c r="G32" t="n">
         <v>90</v>
@@ -1740,10 +1655,7 @@
         <v>297.13</v>
       </c>
       <c r="J32" t="n">
-        <v>150</v>
-      </c>
-      <c r="K32" t="n">
-        <v>2551.868209620667</v>
+        <v>5616.914047610113</v>
       </c>
     </row>
     <row r="33">
@@ -1752,27 +1664,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7b411419-a6bd-5dac-9123-81532f74e720</t>
+          <t>64bccc6b-6f6b-5e1b-865c-149190776323</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Elaine Assis</t>
+          <t>Caio Arruda</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>5960.861253655476</v>
+        <v>8187.839600815882</v>
       </c>
       <c r="F33" t="n">
-        <v>533.99</v>
+        <v>364.76</v>
       </c>
       <c r="G33" t="n">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="H33" t="n">
         <v>254.63</v>
@@ -1781,10 +1693,7 @@
         <v>297.13</v>
       </c>
       <c r="J33" t="n">
-        <v>50</v>
-      </c>
-      <c r="K33" t="n">
-        <v>7186.611253655476</v>
+        <v>9350.35960081588</v>
       </c>
     </row>
     <row r="34">
@@ -1793,12 +1702,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>95042a82-a9a8-552e-98e3-ac15d20bbf2b</t>
+          <t>2bc2241b-333d-5e89-9b7c-7c6524872c01</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Diogo Quintela</t>
+          <t>Camila Dantas</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1807,7 +1716,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1461.243910515265</v>
+        <v>1280.596453813949</v>
       </c>
       <c r="F34" t="n">
         <v>444.99</v>
@@ -1816,16 +1725,13 @@
         <v>90</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I34" t="n">
         <v>297.13</v>
       </c>
       <c r="J34" t="n">
-        <v>50</v>
-      </c>
-      <c r="K34" t="n">
-        <v>2343.363910515265</v>
+        <v>2367.346453813949</v>
       </c>
     </row>
     <row r="35">
@@ -1834,39 +1740,36 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>9ae38b1f-abda-5532-a959-7bfada0e0783</t>
+          <t>52f4cadd-4009-5089-b7fa-65f6e4ab2887</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Daniela Drummond</t>
+          <t>Carlos Magalhães</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>7065.151216079629</v>
+        <v>8837.775201541868</v>
       </c>
       <c r="F35" t="n">
-        <v>684.63</v>
+        <v>364.76</v>
       </c>
       <c r="G35" t="n">
         <v>90</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I35" t="n">
         <v>297.13</v>
       </c>
       <c r="J35" t="n">
-        <v>10</v>
-      </c>
-      <c r="K35" t="n">
-        <v>8146.911216079629</v>
+        <v>9844.295201541867</v>
       </c>
     </row>
     <row r="36">
@@ -1875,12 +1778,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>a0b91621-d2a8-537b-95c4-7ade4c6200ee</t>
+          <t>25f4b46b-119b-54b7-a5fa-03827e5ed16f</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Edson Furtado</t>
+          <t>Carolina Salgado</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1889,13 +1792,13 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>7336.902571199591</v>
+        <v>3266.657357480083</v>
       </c>
       <c r="F36" t="n">
         <v>364.76</v>
       </c>
       <c r="G36" t="n">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1904,10 +1807,7 @@
         <v>297.13</v>
       </c>
       <c r="J36" t="n">
-        <v>50</v>
-      </c>
-      <c r="K36" t="n">
-        <v>8138.792571199591</v>
+        <v>4092.547357480083</v>
       </c>
     </row>
     <row r="37">
@@ -1916,12 +1816,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>a4b3dbb1-86f1-5d25-95a4-82a6c3076da1</t>
+          <t>b298aa3c-d71a-5df0-83c6-312882b5306b</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Alberto da Luz</t>
+          <t>Cássia Tavares</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1930,25 +1830,22 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>7364.526801321949</v>
+        <v>8497.845668097971</v>
       </c>
       <c r="F37" t="n">
-        <v>444.99</v>
+        <v>364.76</v>
       </c>
       <c r="G37" t="n">
         <v>90</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>141.46</v>
       </c>
       <c r="I37" t="n">
         <v>297.13</v>
       </c>
       <c r="J37" t="n">
-        <v>150</v>
-      </c>
-      <c r="K37" t="n">
-        <v>8346.646801321949</v>
+        <v>9391.195668097969</v>
       </c>
     </row>
     <row r="38">
@@ -1957,12 +1854,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>acd778d2-b543-51f4-953c-f9e7e12e7437</t>
+          <t>0eab9fc6-2c73-5288-af73-b13876c87b62</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Benjamin Queiroz</t>
+          <t>Catarina Chaves</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1971,25 +1868,22 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>7920.453739691342</v>
+        <v>3490.64446620121</v>
       </c>
       <c r="F38" t="n">
-        <v>364.76</v>
+        <v>444.99</v>
       </c>
       <c r="G38" t="n">
-        <v>206.57</v>
+        <v>90</v>
       </c>
       <c r="H38" t="n">
-        <v>141.46</v>
+        <v>0</v>
       </c>
       <c r="I38" t="n">
         <v>297.13</v>
       </c>
       <c r="J38" t="n">
-        <v>150</v>
-      </c>
-      <c r="K38" t="n">
-        <v>9080.37373969134</v>
+        <v>4322.76446620121</v>
       </c>
     </row>
     <row r="39">
@@ -1998,21 +1892,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>b1f0b647-06ea-5aaf-9ea0-a84b2b92563f</t>
+          <t>f35e17a9-38ba-5aa7-9a45-c67338c73cc5</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Edite Marinho</t>
+          <t>Célia Lemos</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>800.1804264146962</v>
+        <v>1212.167158944151</v>
       </c>
       <c r="F39" t="n">
         <v>364.76</v>
@@ -2021,16 +1915,13 @@
         <v>90</v>
       </c>
       <c r="H39" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
         <v>297.13</v>
       </c>
       <c r="J39" t="n">
-        <v>50</v>
-      </c>
-      <c r="K39" t="n">
-        <v>1856.700426414696</v>
+        <v>1964.057158944151</v>
       </c>
     </row>
     <row r="40">
@@ -2039,39 +1930,36 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>b298aa3c-d71a-5df0-83c6-312882b5306b</t>
+          <t>3d13f1ba-db27-5fa6-9587-1c539c366638</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cássia Tavares</t>
+          <t>Celso Mourão</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>8497.845668097971</v>
+        <v>257.9421561647101</v>
       </c>
       <c r="F40" t="n">
-        <v>364.76</v>
+        <v>404.91</v>
       </c>
       <c r="G40" t="n">
         <v>90</v>
       </c>
       <c r="H40" t="n">
-        <v>141.46</v>
+        <v>254.63</v>
       </c>
       <c r="I40" t="n">
         <v>297.13</v>
       </c>
       <c r="J40" t="n">
-        <v>10</v>
-      </c>
-      <c r="K40" t="n">
-        <v>9401.195668097969</v>
+        <v>1304.61215616471</v>
       </c>
     </row>
     <row r="41">
@@ -2080,12 +1968,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>b2c05943-feee-5add-9b8e-6bdded9a80a9</t>
+          <t>c57f15e1-0b4a-5ab2-88c8-246678ff4adf</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Beatriz Siqueira</t>
+          <t>César Franco</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2094,10 +1982,10 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>3230.18657849905</v>
+        <v>5902.434171124831</v>
       </c>
       <c r="F41" t="n">
-        <v>533.99</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
         <v>90</v>
@@ -2109,10 +1997,7 @@
         <v>297.13</v>
       </c>
       <c r="J41" t="n">
-        <v>150</v>
-      </c>
-      <c r="K41" t="n">
-        <v>4301.30657849905</v>
+        <v>6289.564171124831</v>
       </c>
     </row>
     <row r="42">
@@ -2121,27 +2006,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>b60d0f65-4360-5bc9-b58b-4056c9de1119</t>
+          <t>d3819e03-5293-5a6a-82ec-d09fd49e456a</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Bianca Saraiva</t>
+          <t>Clarice Barreto</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>6015.101383248207</v>
+        <v>9925.179313508823</v>
       </c>
       <c r="F42" t="n">
         <v>364.76</v>
       </c>
       <c r="G42" t="n">
-        <v>90</v>
+        <v>732</v>
       </c>
       <c r="H42" t="n">
         <v>254.63</v>
@@ -2150,10 +2035,7 @@
         <v>297.13</v>
       </c>
       <c r="J42" t="n">
-        <v>150</v>
-      </c>
-      <c r="K42" t="n">
-        <v>7171.621383248207</v>
+        <v>11573.69931350882</v>
       </c>
     </row>
     <row r="43">
@@ -2162,24 +2044,24 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>b79ce13c-6117-58b6-bc9e-06eaab0a22bb</t>
+          <t>69b08616-ccd0-5227-b382-8bb0265f456f</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Elias Henriques</t>
+          <t>Cláudio Dutra</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>7306.398876912478</v>
+        <v>3997.081814681696</v>
       </c>
       <c r="F43" t="n">
-        <v>-17.8</v>
+        <v>444.99</v>
       </c>
       <c r="G43" t="n">
         <v>90</v>
@@ -2191,10 +2073,7 @@
         <v>297.13</v>
       </c>
       <c r="J43" t="n">
-        <v>50</v>
-      </c>
-      <c r="K43" t="n">
-        <v>7725.728876912478</v>
+        <v>4829.201814681695</v>
       </c>
     </row>
     <row r="44">
@@ -2203,12 +2082,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>b96b9339-e1b9-5d20-b70d-67a8bdb16875</t>
+          <t>f98cdcb6-f68d-5086-b480-7490f8a1675f</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Alan Esteves</t>
+          <t>Cristiano Vasconcelos</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2217,10 +2096,10 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>8059.789738823023</v>
+        <v>5244.95395791246</v>
       </c>
       <c r="F44" t="n">
-        <v>444.99</v>
+        <v>533.99</v>
       </c>
       <c r="G44" t="n">
         <v>90</v>
@@ -2232,10 +2111,7 @@
         <v>297.13</v>
       </c>
       <c r="J44" t="n">
-        <v>150</v>
-      </c>
-      <c r="K44" t="n">
-        <v>9041.909738823022</v>
+        <v>6166.07395791246</v>
       </c>
     </row>
     <row r="45">
@@ -2244,37 +2120,36 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>b9f4ce97-2bdc-5c19-8c35-5db4419b4948</t>
+          <t>3f4a1eeb-c287-57d9-8407-78ea76ba96ea</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bruna Padilha</t>
+          <t>Cristina Meireles</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>7266.55679736717</v>
+        <v>6183.77422031294</v>
       </c>
       <c r="F45" t="n">
-        <v>533.99</v>
+        <v>364.76</v>
       </c>
       <c r="G45" t="n">
         <v>90</v>
       </c>
       <c r="H45" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
         <v>297.13</v>
       </c>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="n">
-        <v>8442.30679736717</v>
+      <c r="J45" t="n">
+        <v>6935.66422031294</v>
       </c>
     </row>
     <row r="46">
@@ -2283,39 +2158,36 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>c4998a9b-cc38-5851-9223-7cf43ea91c36</t>
+          <t>da7b82a2-d4bc-5993-8e5f-59aa3081241a</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Alice Farias</t>
+          <t>Daniel Bezerra</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>8284.136836853117</v>
+        <v>6173.403303137569</v>
       </c>
       <c r="F46" t="n">
-        <v>560.7</v>
+        <v>444.99</v>
       </c>
       <c r="G46" t="n">
         <v>90</v>
       </c>
       <c r="H46" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
         <v>297.13</v>
       </c>
       <c r="J46" t="n">
-        <v>150</v>
-      </c>
-      <c r="K46" t="n">
-        <v>9636.596836853116</v>
+        <v>7005.523303137569</v>
       </c>
     </row>
     <row r="47">
@@ -2324,24 +2196,24 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>c4fd9f54-9504-52b3-9fca-ab39c50dc07f</t>
+          <t>9ae38b1f-abda-5532-a959-7bfada0e0783</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Anselmo Novaes</t>
+          <t>Daniela Drummond</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>1108.340345861018</v>
+        <v>7065.151216079629</v>
       </c>
       <c r="F47" t="n">
-        <v>444.99</v>
+        <v>684.63</v>
       </c>
       <c r="G47" t="n">
         <v>90</v>
@@ -2353,10 +2225,7 @@
         <v>297.13</v>
       </c>
       <c r="J47" t="n">
-        <v>150</v>
-      </c>
-      <c r="K47" t="n">
-        <v>2090.460345861018</v>
+        <v>8136.911216079629</v>
       </c>
     </row>
     <row r="48">
@@ -2365,12 +2234,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>c57f15e1-0b4a-5ab2-88c8-246678ff4adf</t>
+          <t>06be0738-b15f-5d07-892b-d45971647c79</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>César Franco</t>
+          <t>Danilo Brandão</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2379,10 +2248,10 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5902.434171124831</v>
+        <v>9095.090151715545</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>855.8</v>
       </c>
       <c r="G48" t="n">
         <v>90</v>
@@ -2394,10 +2263,7 @@
         <v>297.13</v>
       </c>
       <c r="J48" t="n">
-        <v>10</v>
-      </c>
-      <c r="K48" t="n">
-        <v>6299.564171124831</v>
+        <v>10338.02015171554</v>
       </c>
     </row>
     <row r="49">
@@ -2406,27 +2272,27 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>c8fdc760-5724-5f8c-82ae-2e6e767b3811</t>
+          <t>ec7d2162-5de8-50e9-9aea-a1dd90ec8081</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Denis Macedo</t>
+          <t>Davi Caldeira</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>3952.204962932551</v>
+        <v>746.9510783679258</v>
       </c>
       <c r="F49" t="n">
-        <v>364.76</v>
+        <v>560.7</v>
       </c>
       <c r="G49" t="n">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="H49" t="n">
         <v>254.63</v>
@@ -2434,9 +2300,8 @@
       <c r="I49" t="n">
         <v>297.13</v>
       </c>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="n">
-        <v>5032.724962932551</v>
+      <c r="J49" t="n">
+        <v>1949.411078367926</v>
       </c>
     </row>
     <row r="50">
@@ -2445,24 +2310,24 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ca2f5a2d-c388-5837-ae1f-93173331ba9a</t>
+          <t>ca78df0b-cb88-5905-ab6f-c47150af2c20</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Alexandre da Mata</t>
+          <t>Débora Guedes</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>9551.21905794158</v>
+        <v>8733.661290965678</v>
       </c>
       <c r="F50" t="n">
-        <v>364.76</v>
+        <v>855.8</v>
       </c>
       <c r="G50" t="n">
         <v>90</v>
@@ -2474,10 +2339,7 @@
         <v>297.13</v>
       </c>
       <c r="J50" t="n">
-        <v>150</v>
-      </c>
-      <c r="K50" t="n">
-        <v>10707.73905794158</v>
+        <v>10231.22129096568</v>
       </c>
     </row>
     <row r="51">
@@ -2486,27 +2348,27 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ca78df0b-cb88-5905-ab6f-c47150af2c20</t>
+          <t>c8fdc760-5724-5f8c-82ae-2e6e767b3811</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Débora Guedes</t>
+          <t>Denis Macedo</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>8733.661290965678</v>
+        <v>3952.204962932551</v>
       </c>
       <c r="F51" t="n">
-        <v>855.8</v>
+        <v>364.76</v>
       </c>
       <c r="G51" t="n">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="H51" t="n">
         <v>254.63</v>
@@ -2515,10 +2377,7 @@
         <v>297.13</v>
       </c>
       <c r="J51" t="n">
-        <v>10</v>
-      </c>
-      <c r="K51" t="n">
-        <v>10241.22129096568</v>
+        <v>5032.724962932551</v>
       </c>
     </row>
     <row r="52">
@@ -2527,12 +2386,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ce6652c4-e8d1-5805-81c2-2fdc603f51b0</t>
+          <t>17533122-8361-509c-9e67-8887db2e0001</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Antônio Viana</t>
+          <t>Diana Azevedo</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2541,25 +2400,22 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>3295.032751492262</v>
+        <v>6993.13850131002</v>
       </c>
       <c r="F52" t="n">
-        <v>560.7</v>
+        <v>-328.28</v>
       </c>
       <c r="G52" t="n">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="H52" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>297.13</v>
       </c>
       <c r="J52" t="n">
-        <v>150</v>
-      </c>
-      <c r="K52" t="n">
-        <v>4674.492751492262</v>
+        <v>7708.54850131002</v>
       </c>
     </row>
     <row r="53">
@@ -2568,27 +2424,27 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>d3819e03-5293-5a6a-82ec-d09fd49e456a</t>
+          <t>4b86c62c-6ddf-539d-ac69-cc6cc522386a</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Clarice Barreto</t>
+          <t>Diego Figueiredo</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>G&amp;A</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>9925.179313508823</v>
+        <v>490.174359132607</v>
       </c>
       <c r="F53" t="n">
-        <v>364.76</v>
+        <v>622.41</v>
       </c>
       <c r="G53" t="n">
-        <v>732</v>
+        <v>90</v>
       </c>
       <c r="H53" t="n">
         <v>254.63</v>
@@ -2597,10 +2453,7 @@
         <v>297.13</v>
       </c>
       <c r="J53" t="n">
-        <v>10</v>
-      </c>
-      <c r="K53" t="n">
-        <v>11583.69931350882</v>
+        <v>1754.344359132607</v>
       </c>
     </row>
     <row r="54">
@@ -2609,12 +2462,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>d4d9f427-c9cd-5935-a88d-60bb469e7c89</t>
+          <t>95042a82-a9a8-552e-98e3-ac15d20bbf2b</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Álvaro da Paz</t>
+          <t>Diogo Quintela</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2623,25 +2476,22 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1223.312552727439</v>
+        <v>1461.243910515265</v>
       </c>
       <c r="F54" t="n">
-        <v>533.99</v>
+        <v>444.99</v>
       </c>
       <c r="G54" t="n">
         <v>90</v>
       </c>
       <c r="H54" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
         <v>297.13</v>
       </c>
       <c r="J54" t="n">
-        <v>150</v>
-      </c>
-      <c r="K54" t="n">
-        <v>2549.062552727439</v>
+        <v>2293.363910515265</v>
       </c>
     </row>
     <row r="55">
@@ -2650,21 +2500,21 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>d5426380-369f-500b-a136-ce5543c13c0d</t>
+          <t>7339364e-8890-571d-86f0-ddf62dd4b918</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Edgar Cordeiro</t>
+          <t>Douglas Sardinha</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>4455.059040524839</v>
+        <v>2741.365342728207</v>
       </c>
       <c r="F55" t="n">
         <v>444.99</v>
@@ -2679,10 +2529,7 @@
         <v>297.13</v>
       </c>
       <c r="J55" t="n">
-        <v>50</v>
-      </c>
-      <c r="K55" t="n">
-        <v>5337.179040524838</v>
+        <v>3573.485342728207</v>
       </c>
     </row>
     <row r="56">
@@ -2691,12 +2538,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>da7b82a2-d4bc-5993-8e5f-59aa3081241a</t>
+          <t>d5426380-369f-500b-a136-ce5543c13c0d</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Daniel Bezerra</t>
+          <t>Edgar Cordeiro</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2705,7 +2552,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>6173.403303137569</v>
+        <v>4455.059040524839</v>
       </c>
       <c r="F56" t="n">
         <v>444.99</v>
@@ -2720,10 +2567,7 @@
         <v>297.13</v>
       </c>
       <c r="J56" t="n">
-        <v>10</v>
-      </c>
-      <c r="K56" t="n">
-        <v>7015.523303137569</v>
+        <v>5287.179040524838</v>
       </c>
     </row>
     <row r="57">
@@ -2732,24 +2576,24 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>db0b9e18-aa43-5a04-b686-ac454728ad3a</t>
+          <t>b1f0b647-06ea-5aaf-9ea0-a84b2b92563f</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Elielson Quadros</t>
+          <t>Edite Marinho</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6715.641722399166</v>
+        <v>800.1804264146962</v>
       </c>
       <c r="F57" t="n">
-        <v>498.39</v>
+        <v>364.76</v>
       </c>
       <c r="G57" t="n">
         <v>90</v>
@@ -2760,9 +2604,8 @@
       <c r="I57" t="n">
         <v>297.13</v>
       </c>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="n">
-        <v>7855.791722399166</v>
+      <c r="J57" t="n">
+        <v>1806.700426414696</v>
       </c>
     </row>
     <row r="58">
@@ -2771,12 +2614,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ea3147dc-902e-5ded-88e8-10514c53e142</t>
+          <t>a0b91621-d2a8-537b-95c4-7ade4c6200ee</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Ana Melo</t>
+          <t>Edson Furtado</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2785,10 +2628,10 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>8057.257421621038</v>
+        <v>7336.902571199591</v>
       </c>
       <c r="F58" t="n">
-        <v>444.99</v>
+        <v>364.76</v>
       </c>
       <c r="G58" t="n">
         <v>90</v>
@@ -2800,10 +2643,7 @@
         <v>297.13</v>
       </c>
       <c r="J58" t="n">
-        <v>150</v>
-      </c>
-      <c r="K58" t="n">
-        <v>9039.377421621037</v>
+        <v>8088.792571199591</v>
       </c>
     </row>
     <row r="59">
@@ -2812,12 +2652,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ec7d2162-5de8-50e9-9aea-a1dd90ec8081</t>
+          <t>2c297031-afd1-540c-a226-32291c3b420d</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Davi Caldeira</t>
+          <t>Eduardo Portela</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2826,25 +2666,22 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>746.9510783679258</v>
+        <v>1728.629771639805</v>
       </c>
       <c r="F59" t="n">
         <v>560.7</v>
       </c>
       <c r="G59" t="n">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="H59" t="n">
-        <v>254.63</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>297.13</v>
       </c>
       <c r="J59" t="n">
-        <v>10</v>
-      </c>
-      <c r="K59" t="n">
-        <v>1959.411078367926</v>
+        <v>2703.459771639805</v>
       </c>
     </row>
     <row r="60">
@@ -2853,39 +2690,36 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>f08290a7-3372-5637-9244-a80f8bc9ee3c</t>
+          <t>7b411419-a6bd-5dac-9123-81532f74e720</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Ângela Rezende</t>
+          <t>Elaine Assis</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>COGS</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>2036.514997025348</v>
+        <v>5960.861253655476</v>
       </c>
       <c r="F60" t="n">
-        <v>364.76</v>
+        <v>533.99</v>
       </c>
       <c r="G60" t="n">
         <v>90</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I60" t="n">
         <v>297.13</v>
       </c>
       <c r="J60" t="n">
-        <v>150</v>
-      </c>
-      <c r="K60" t="n">
-        <v>2938.404997025348</v>
+        <v>7136.611253655476</v>
       </c>
     </row>
     <row r="61">
@@ -2894,12 +2728,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>f35e17a9-38ba-5aa7-9a45-c67338c73cc5</t>
+          <t>b79ce13c-6117-58b6-bc9e-06eaab0a22bb</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Célia Lemos</t>
+          <t>Elias Henriques</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2908,10 +2742,10 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1212.167158944151</v>
+        <v>7306.398876912478</v>
       </c>
       <c r="F61" t="n">
-        <v>364.76</v>
+        <v>-17.8</v>
       </c>
       <c r="G61" t="n">
         <v>90</v>
@@ -2923,10 +2757,7 @@
         <v>297.13</v>
       </c>
       <c r="J61" t="n">
-        <v>10</v>
-      </c>
-      <c r="K61" t="n">
-        <v>1974.057158944151</v>
+        <v>7711.328876912478</v>
       </c>
     </row>
     <row r="62">
@@ -2935,21 +2766,21 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>f98cdcb6-f68d-5086-b480-7490f8a1675f</t>
+          <t>61a920cf-a29d-5536-a8ab-3f23dcee4a4b</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Cristiano Vasconcelos</t>
+          <t>Eliane Jurema</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>R&amp;D</t>
+          <t>COGS</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>5244.95395791246</v>
+        <v>4055.50889721234</v>
       </c>
       <c r="F62" t="n">
         <v>533.99</v>
@@ -2958,16 +2789,13 @@
         <v>90</v>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>254.63</v>
       </c>
       <c r="I62" t="n">
         <v>297.13</v>
       </c>
       <c r="J62" t="n">
-        <v>10</v>
-      </c>
-      <c r="K62" t="n">
-        <v>6176.07395791246</v>
+        <v>5231.25889721234</v>
       </c>
     </row>
     <row r="63">
@@ -2976,58 +2804,36 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>f9e02392-bc91-5868-91d5-4a90ccc2cbbf</t>
+          <t>db0b9e18-aa43-5a04-b686-ac454728ad3a</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Anderson Aragão</t>
+          <t>Elielson Quadros</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>G&amp;A</t>
+          <t>R&amp;D</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>9712.728285382607</v>
+        <v>6715.641722399166</v>
       </c>
       <c r="F63" t="n">
-        <v>533.99</v>
+        <v>498.39</v>
       </c>
       <c r="G63" t="n">
         <v>90</v>
       </c>
       <c r="H63" t="n">
-        <v>141.46</v>
+        <v>254.63</v>
       </c>
       <c r="I63" t="n">
         <v>297.13</v>
       </c>
       <c r="J63" t="n">
-        <v>150</v>
-      </c>
-      <c r="K63" t="n">
-        <v>10925.30828538261</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="n">
-        <v>50</v>
-      </c>
-      <c r="K64" t="n">
-        <v>50</v>
+        <v>7855.791722399166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>